<commit_message>
change valuation terminal value
</commit_message>
<xml_diff>
--- a/database/industries/ghaza/gheshasfa/balancesheet/yearly.xlsx
+++ b/database/industries/ghaza/gheshasfa/balancesheet/yearly.xlsx
@@ -192,6 +192,11 @@
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="29" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
+    <col min="12" max="12" width="29" customWidth="1"/>
+    <col min="13" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -216,6 +221,21 @@
       <c r="H1" s="2">
         <v/>
       </c>
+      <c r="I1" s="2">
+        <v/>
+      </c>
+      <c r="J1" s="2">
+        <v/>
+      </c>
+      <c r="K1" s="2">
+        <v/>
+      </c>
+      <c r="L1" s="2">
+        <v/>
+      </c>
+      <c r="M1" s="2">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="3" t="inlineStr">
@@ -241,6 +261,21 @@
       <c r="H2" s="2">
         <v/>
       </c>
+      <c r="I2" s="2">
+        <v/>
+      </c>
+      <c r="J2" s="2">
+        <v/>
+      </c>
+      <c r="K2" s="2">
+        <v/>
+      </c>
+      <c r="L2" s="2">
+        <v/>
+      </c>
+      <c r="M2" s="2">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="4" t="inlineStr">
@@ -266,6 +301,21 @@
       <c r="H3" s="2">
         <v/>
       </c>
+      <c r="I3" s="2">
+        <v/>
+      </c>
+      <c r="J3" s="2">
+        <v/>
+      </c>
+      <c r="K3" s="2">
+        <v/>
+      </c>
+      <c r="L3" s="2">
+        <v/>
+      </c>
+      <c r="M3" s="2">
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="2">
@@ -289,6 +339,21 @@
       <c r="H4" s="2">
         <v/>
       </c>
+      <c r="I4" s="2">
+        <v/>
+      </c>
+      <c r="J4" s="2">
+        <v/>
+      </c>
+      <c r="K4" s="2">
+        <v/>
+      </c>
+      <c r="L4" s="2">
+        <v/>
+      </c>
+      <c r="M4" s="2">
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="5" t="inlineStr">
@@ -314,6 +379,21 @@
       <c r="H5" s="5">
         <v/>
       </c>
+      <c r="I5" s="5">
+        <v/>
+      </c>
+      <c r="J5" s="5">
+        <v/>
+      </c>
+      <c r="K5" s="5">
+        <v/>
+      </c>
+      <c r="L5" s="5">
+        <v/>
+      </c>
+      <c r="M5" s="5">
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="6" t="inlineStr">
@@ -339,6 +419,21 @@
       <c r="H6" s="5">
         <v/>
       </c>
+      <c r="I6" s="5">
+        <v/>
+      </c>
+      <c r="J6" s="5">
+        <v/>
+      </c>
+      <c r="K6" s="5">
+        <v/>
+      </c>
+      <c r="L6" s="5">
+        <v/>
+      </c>
+      <c r="M6" s="5">
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="2">
@@ -362,6 +457,21 @@
       <c r="H7" s="2">
         <v/>
       </c>
+      <c r="I7" s="2">
+        <v/>
+      </c>
+      <c r="J7" s="2">
+        <v/>
+      </c>
+      <c r="K7" s="2">
+        <v/>
+      </c>
+      <c r="L7" s="2">
+        <v/>
+      </c>
+      <c r="M7" s="2">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="8" t="inlineStr">
@@ -374,25 +484,50 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
+          <t>12 ماهه منتهی به 1391/12</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1392/12</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1393/12</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1394/12</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1395/12</t>
+        </is>
+      </c>
+      <c r="I8" s="7" t="inlineStr">
+        <is>
           <t>12 ماهه منتهی به 1396/12</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
+      <c r="J8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1397/12</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr">
+      <c r="K8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1398/12</t>
         </is>
       </c>
-      <c r="G8" s="7" t="inlineStr">
+      <c r="L8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1399/12</t>
         </is>
       </c>
-      <c r="H8" s="7" t="inlineStr">
+      <c r="M8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1400/12</t>
         </is>
@@ -409,27 +544,52 @@
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
+          <t>1393-02-21 (7)</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="inlineStr">
+        <is>
+          <t>1394-02-24 (9)</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="inlineStr">
+        <is>
+          <t>1395-02-25 (8)</t>
+        </is>
+      </c>
+      <c r="G9" s="10" t="inlineStr">
+        <is>
+          <t>1396-02-21 (9)</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>1397-04-09 (11)</t>
+        </is>
+      </c>
+      <c r="I9" s="10" t="inlineStr">
+        <is>
           <t>1398-02-22 (9)</t>
         </is>
       </c>
-      <c r="E9" s="10" t="inlineStr">
+      <c r="J9" s="10" t="inlineStr">
         <is>
           <t>1399-02-14 (8)</t>
         </is>
       </c>
-      <c r="F9" s="10" t="inlineStr">
+      <c r="K9" s="10" t="inlineStr">
         <is>
           <t>1400-02-21 (8)</t>
         </is>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="L9" s="10" t="inlineStr">
         <is>
           <t>1401-02-18 (9)</t>
         </is>
       </c>
-      <c r="H9" s="10" t="inlineStr">
-        <is>
-          <t>1401-04-28 (3)</t>
+      <c r="M9" s="10" t="inlineStr">
+        <is>
+          <t>1401-08-09 (5)</t>
         </is>
       </c>
     </row>
@@ -455,6 +615,21 @@
       <c r="H10" s="12">
         <v/>
       </c>
+      <c r="I10" s="12">
+        <v/>
+      </c>
+      <c r="J10" s="12">
+        <v/>
+      </c>
+      <c r="K10" s="12">
+        <v/>
+      </c>
+      <c r="L10" s="12">
+        <v/>
+      </c>
+      <c r="M10" s="12">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -480,6 +655,21 @@
       <c r="H11" s="14">
         <v/>
       </c>
+      <c r="I11" s="14">
+        <v/>
+      </c>
+      <c r="J11" s="14">
+        <v/>
+      </c>
+      <c r="K11" s="14">
+        <v/>
+      </c>
+      <c r="L11" s="14">
+        <v/>
+      </c>
+      <c r="M11" s="14">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="15" t="inlineStr">
@@ -491,18 +681,33 @@
         <v/>
       </c>
       <c r="D12" s="16">
+        <v>39104</v>
+      </c>
+      <c r="E12" s="16">
+        <v>9251</v>
+      </c>
+      <c r="F12" s="16">
+        <v>8986</v>
+      </c>
+      <c r="G12" s="16">
+        <v>9042</v>
+      </c>
+      <c r="H12" s="16">
+        <v>5920</v>
+      </c>
+      <c r="I12" s="16">
         <v>5827</v>
       </c>
-      <c r="E12" s="16">
+      <c r="J12" s="16">
         <v>20276</v>
       </c>
-      <c r="F12" s="16">
+      <c r="K12" s="16">
         <v>138068</v>
       </c>
-      <c r="G12" s="16">
+      <c r="L12" s="16">
         <v>100125</v>
       </c>
-      <c r="H12" s="16">
+      <c r="M12" s="16">
         <v>198752</v>
       </c>
     </row>
@@ -516,18 +721,33 @@
         <v/>
       </c>
       <c r="D13" s="12">
+        <v>39</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>28888</v>
+      </c>
+      <c r="H13" s="12">
+        <v>19787</v>
+      </c>
+      <c r="I13" s="12">
         <v>15000</v>
       </c>
-      <c r="E13" s="12">
+      <c r="J13" s="12">
         <v>25000</v>
       </c>
-      <c r="F13" s="12">
+      <c r="K13" s="12">
         <v>25000</v>
       </c>
-      <c r="G13" s="12">
-        <v>0</v>
-      </c>
-      <c r="H13" s="12">
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
         <v>0</v>
       </c>
     </row>
@@ -541,18 +761,33 @@
         <v/>
       </c>
       <c r="D14" s="16">
+        <v>159220</v>
+      </c>
+      <c r="E14" s="16">
+        <v>214732</v>
+      </c>
+      <c r="F14" s="16">
+        <v>249053</v>
+      </c>
+      <c r="G14" s="16">
+        <v>351818</v>
+      </c>
+      <c r="H14" s="16">
+        <v>589895</v>
+      </c>
+      <c r="I14" s="16">
         <v>646524</v>
       </c>
-      <c r="E14" s="16">
+      <c r="J14" s="16">
         <v>798236</v>
       </c>
-      <c r="F14" s="16">
+      <c r="K14" s="16">
         <v>819086</v>
       </c>
-      <c r="G14" s="16">
+      <c r="L14" s="16">
         <v>963838</v>
       </c>
-      <c r="H14" s="16">
+      <c r="M14" s="16">
         <v>1187266</v>
       </c>
     </row>
@@ -566,18 +801,33 @@
         <v/>
       </c>
       <c r="D15" s="12">
+        <v>167977</v>
+      </c>
+      <c r="E15" s="12">
+        <v>229816</v>
+      </c>
+      <c r="F15" s="12">
+        <v>188059</v>
+      </c>
+      <c r="G15" s="12">
+        <v>243753</v>
+      </c>
+      <c r="H15" s="12">
+        <v>279595</v>
+      </c>
+      <c r="I15" s="12">
         <v>323821</v>
       </c>
-      <c r="E15" s="12">
+      <c r="J15" s="12">
         <v>625667</v>
       </c>
-      <c r="F15" s="12">
+      <c r="K15" s="12">
         <v>1281808</v>
       </c>
-      <c r="G15" s="12">
+      <c r="L15" s="12">
         <v>1883039</v>
       </c>
-      <c r="H15" s="12">
+      <c r="M15" s="12">
         <v>2811302</v>
       </c>
     </row>
@@ -591,18 +841,33 @@
         <v/>
       </c>
       <c r="D16" s="16">
+        <v>5671</v>
+      </c>
+      <c r="E16" s="16">
+        <v>12963</v>
+      </c>
+      <c r="F16" s="16">
+        <v>8416</v>
+      </c>
+      <c r="G16" s="16">
+        <v>9482</v>
+      </c>
+      <c r="H16" s="16">
+        <v>12014</v>
+      </c>
+      <c r="I16" s="16">
         <v>5668</v>
       </c>
-      <c r="E16" s="16">
+      <c r="J16" s="16">
         <v>18914</v>
       </c>
-      <c r="F16" s="16">
+      <c r="K16" s="16">
         <v>29304</v>
       </c>
-      <c r="G16" s="16">
+      <c r="L16" s="16">
         <v>30341</v>
       </c>
-      <c r="H16" s="16">
+      <c r="M16" s="16">
         <v>43618</v>
       </c>
     </row>
@@ -625,9 +890,24 @@
         <v>0</v>
       </c>
       <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
         <v>2878</v>
       </c>
-      <c r="H17" s="12">
+      <c r="M17" s="12">
         <v>2878</v>
       </c>
     </row>
@@ -641,18 +921,33 @@
         <v/>
       </c>
       <c r="D18" s="18">
+        <v>372011</v>
+      </c>
+      <c r="E18" s="18">
+        <v>466762</v>
+      </c>
+      <c r="F18" s="18">
+        <v>454514</v>
+      </c>
+      <c r="G18" s="18">
+        <v>642983</v>
+      </c>
+      <c r="H18" s="18">
+        <v>907211</v>
+      </c>
+      <c r="I18" s="18">
         <v>996840</v>
       </c>
-      <c r="E18" s="18">
+      <c r="J18" s="18">
         <v>1488093</v>
       </c>
-      <c r="F18" s="18">
+      <c r="K18" s="18">
         <v>2293266</v>
       </c>
-      <c r="G18" s="18">
+      <c r="L18" s="18">
         <v>2980221</v>
       </c>
-      <c r="H18" s="18">
+      <c r="M18" s="18">
         <v>4243816</v>
       </c>
     </row>
@@ -666,18 +961,33 @@
         <v/>
       </c>
       <c r="D19" s="12">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12">
+        <v>1400</v>
+      </c>
+      <c r="G19" s="12">
+        <v>4700</v>
+      </c>
+      <c r="H19" s="12">
+        <v>4440</v>
+      </c>
+      <c r="I19" s="12">
         <v>4427</v>
       </c>
-      <c r="E19" s="12">
+      <c r="J19" s="12">
         <v>4751</v>
       </c>
-      <c r="F19" s="12">
+      <c r="K19" s="12">
         <v>7041</v>
       </c>
-      <c r="G19" s="12">
+      <c r="L19" s="12">
         <v>7306</v>
       </c>
-      <c r="H19" s="12">
+      <c r="M19" s="12">
         <v>7290</v>
       </c>
     </row>
@@ -694,15 +1004,30 @@
         <v>332</v>
       </c>
       <c r="E20" s="16">
+        <v>2332</v>
+      </c>
+      <c r="F20" s="16">
+        <v>17332</v>
+      </c>
+      <c r="G20" s="16">
+        <v>15332</v>
+      </c>
+      <c r="H20" s="16">
+        <v>15332</v>
+      </c>
+      <c r="I20" s="16">
+        <v>332</v>
+      </c>
+      <c r="J20" s="16">
         <v>335</v>
       </c>
-      <c r="F20" s="16">
+      <c r="K20" s="16">
         <v>335</v>
       </c>
-      <c r="G20" s="16">
+      <c r="L20" s="16">
         <v>335</v>
       </c>
-      <c r="H20" s="16">
+      <c r="M20" s="16">
         <v>335</v>
       </c>
     </row>
@@ -715,19 +1040,40 @@
       <c r="C21" s="12">
         <v/>
       </c>
-      <c r="D21" s="12">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12">
-        <v>0</v>
-      </c>
-      <c r="F21" s="12">
-        <v>0</v>
+      <c r="D21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G21" s="12">
         <v>0</v>
       </c>
       <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12">
         <v>0</v>
       </c>
     </row>
@@ -741,18 +1087,33 @@
         <v/>
       </c>
       <c r="D22" s="16">
+        <v>150190</v>
+      </c>
+      <c r="E22" s="16">
+        <v>151261</v>
+      </c>
+      <c r="F22" s="16">
+        <v>161426</v>
+      </c>
+      <c r="G22" s="16">
+        <v>167406</v>
+      </c>
+      <c r="H22" s="16">
+        <v>194266</v>
+      </c>
+      <c r="I22" s="16">
         <v>217665</v>
       </c>
-      <c r="E22" s="16">
+      <c r="J22" s="16">
         <v>334281</v>
       </c>
-      <c r="F22" s="16">
+      <c r="K22" s="16">
         <v>1196273</v>
       </c>
-      <c r="G22" s="16">
+      <c r="L22" s="16">
         <v>1880501</v>
       </c>
-      <c r="H22" s="16">
+      <c r="M22" s="16">
         <v>3037202</v>
       </c>
     </row>
@@ -766,18 +1127,33 @@
         <v/>
       </c>
       <c r="D23" s="12">
-        <v>414</v>
+        <v>197</v>
       </c>
       <c r="E23" s="12">
-        <v>389</v>
+        <v>197</v>
       </c>
       <c r="F23" s="12">
         <v>381</v>
       </c>
       <c r="G23" s="12">
+        <v>421</v>
+      </c>
+      <c r="H23" s="12">
+        <v>439</v>
+      </c>
+      <c r="I23" s="12">
+        <v>414</v>
+      </c>
+      <c r="J23" s="12">
+        <v>389</v>
+      </c>
+      <c r="K23" s="12">
+        <v>381</v>
+      </c>
+      <c r="L23" s="12">
         <v>17504</v>
       </c>
-      <c r="H23" s="12">
+      <c r="M23" s="12">
         <v>17504</v>
       </c>
     </row>
@@ -790,15 +1166,11 @@
       <c r="C24" s="16">
         <v/>
       </c>
-      <c r="D24" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>0</v>
       </c>
       <c r="F24" s="16" t="inlineStr">
         <is>
@@ -811,6 +1183,31 @@
         </is>
       </c>
       <c r="H24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M24" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -826,18 +1223,33 @@
         <v/>
       </c>
       <c r="D25" s="12">
+        <v>13569</v>
+      </c>
+      <c r="E25" s="12">
+        <v>18927</v>
+      </c>
+      <c r="F25" s="12">
+        <v>9277</v>
+      </c>
+      <c r="G25" s="12">
+        <v>9650</v>
+      </c>
+      <c r="H25" s="12">
+        <v>9545</v>
+      </c>
+      <c r="I25" s="12">
         <v>5350</v>
       </c>
-      <c r="E25" s="12">
+      <c r="J25" s="12">
         <v>5350</v>
       </c>
-      <c r="F25" s="12">
+      <c r="K25" s="12">
         <v>1100</v>
       </c>
-      <c r="G25" s="12">
+      <c r="L25" s="12">
         <v>1100</v>
       </c>
-      <c r="H25" s="12">
+      <c r="M25" s="12">
         <v>1100</v>
       </c>
     </row>
@@ -851,18 +1263,33 @@
         <v/>
       </c>
       <c r="D26" s="18">
+        <v>164288</v>
+      </c>
+      <c r="E26" s="18">
+        <v>172717</v>
+      </c>
+      <c r="F26" s="18">
+        <v>189816</v>
+      </c>
+      <c r="G26" s="18">
+        <v>197509</v>
+      </c>
+      <c r="H26" s="18">
+        <v>224022</v>
+      </c>
+      <c r="I26" s="18">
         <v>228188</v>
       </c>
-      <c r="E26" s="18">
+      <c r="J26" s="18">
         <v>345106</v>
       </c>
-      <c r="F26" s="18">
+      <c r="K26" s="18">
         <v>1205130</v>
       </c>
-      <c r="G26" s="18">
+      <c r="L26" s="18">
         <v>1906746</v>
       </c>
-      <c r="H26" s="18">
+      <c r="M26" s="18">
         <v>3063431</v>
       </c>
     </row>
@@ -876,18 +1303,33 @@
         <v/>
       </c>
       <c r="D27" s="20">
+        <v>536299</v>
+      </c>
+      <c r="E27" s="20">
+        <v>639479</v>
+      </c>
+      <c r="F27" s="20">
+        <v>644330</v>
+      </c>
+      <c r="G27" s="20">
+        <v>840492</v>
+      </c>
+      <c r="H27" s="20">
+        <v>1131233</v>
+      </c>
+      <c r="I27" s="20">
         <v>1225028</v>
       </c>
-      <c r="E27" s="20">
+      <c r="J27" s="20">
         <v>1833199</v>
       </c>
-      <c r="F27" s="20">
+      <c r="K27" s="20">
         <v>3498396</v>
       </c>
-      <c r="G27" s="20">
+      <c r="L27" s="20">
         <v>4886967</v>
       </c>
-      <c r="H27" s="20">
+      <c r="M27" s="20">
         <v>7307247</v>
       </c>
     </row>
@@ -915,6 +1357,21 @@
       <c r="H28" s="14">
         <v/>
       </c>
+      <c r="I28" s="14">
+        <v/>
+      </c>
+      <c r="J28" s="14">
+        <v/>
+      </c>
+      <c r="K28" s="14">
+        <v/>
+      </c>
+      <c r="L28" s="14">
+        <v/>
+      </c>
+      <c r="M28" s="14">
+        <v/>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="15" t="inlineStr">
@@ -926,18 +1383,33 @@
         <v/>
       </c>
       <c r="D29" s="16">
+        <v>231670</v>
+      </c>
+      <c r="E29" s="16">
+        <v>285979</v>
+      </c>
+      <c r="F29" s="16">
+        <v>253135</v>
+      </c>
+      <c r="G29" s="16">
+        <v>448180</v>
+      </c>
+      <c r="H29" s="16">
+        <v>531885</v>
+      </c>
+      <c r="I29" s="16">
         <v>606722</v>
       </c>
-      <c r="E29" s="16">
+      <c r="J29" s="16">
         <v>891878</v>
       </c>
-      <c r="F29" s="16">
+      <c r="K29" s="16">
         <v>1657728</v>
       </c>
-      <c r="G29" s="16">
+      <c r="L29" s="16">
         <v>2196236</v>
       </c>
-      <c r="H29" s="16">
+      <c r="M29" s="16">
         <v>3562927</v>
       </c>
     </row>
@@ -950,15 +1422,11 @@
       <c r="C30" s="12">
         <v/>
       </c>
-      <c r="D30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D30" s="12">
+        <v>17703</v>
+      </c>
+      <c r="E30" s="12">
+        <v>30422</v>
       </c>
       <c r="F30" s="12" t="inlineStr">
         <is>
@@ -971,6 +1439,31 @@
         </is>
       </c>
       <c r="H30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M30" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -998,6 +1491,21 @@
         <v>0</v>
       </c>
       <c r="H31" s="16">
+        <v>0</v>
+      </c>
+      <c r="I31" s="16">
+        <v>0</v>
+      </c>
+      <c r="J31" s="16">
+        <v>0</v>
+      </c>
+      <c r="K31" s="16">
+        <v>0</v>
+      </c>
+      <c r="L31" s="16">
+        <v>0</v>
+      </c>
+      <c r="M31" s="16">
         <v>133207</v>
       </c>
     </row>
@@ -1011,18 +1519,33 @@
         <v/>
       </c>
       <c r="D32" s="12">
+        <v>24101</v>
+      </c>
+      <c r="E32" s="12">
+        <v>19026</v>
+      </c>
+      <c r="F32" s="12">
+        <v>31866</v>
+      </c>
+      <c r="G32" s="12">
+        <v>37339</v>
+      </c>
+      <c r="H32" s="12">
+        <v>44623</v>
+      </c>
+      <c r="I32" s="12">
         <v>55439</v>
       </c>
-      <c r="E32" s="12">
+      <c r="J32" s="12">
         <v>67578</v>
       </c>
-      <c r="F32" s="12">
+      <c r="K32" s="12">
         <v>116057</v>
       </c>
-      <c r="G32" s="12">
+      <c r="L32" s="12">
         <v>208869</v>
       </c>
-      <c r="H32" s="12">
+      <c r="M32" s="12">
         <v>287962</v>
       </c>
     </row>
@@ -1036,18 +1559,33 @@
         <v/>
       </c>
       <c r="D33" s="16">
+        <v>4067</v>
+      </c>
+      <c r="E33" s="16">
+        <v>7822</v>
+      </c>
+      <c r="F33" s="16">
+        <v>9931</v>
+      </c>
+      <c r="G33" s="16">
+        <v>8802</v>
+      </c>
+      <c r="H33" s="16">
+        <v>5527</v>
+      </c>
+      <c r="I33" s="16">
         <v>13449</v>
       </c>
-      <c r="E33" s="16">
+      <c r="J33" s="16">
         <v>33627</v>
       </c>
-      <c r="F33" s="16">
+      <c r="K33" s="16">
         <v>20428</v>
       </c>
-      <c r="G33" s="16">
+      <c r="L33" s="16">
         <v>53904</v>
       </c>
-      <c r="H33" s="16">
+      <c r="M33" s="16">
         <v>40452</v>
       </c>
     </row>
@@ -1061,18 +1599,33 @@
         <v/>
       </c>
       <c r="D34" s="12">
+        <v>66526</v>
+      </c>
+      <c r="E34" s="12">
+        <v>119265</v>
+      </c>
+      <c r="F34" s="12">
+        <v>128259</v>
+      </c>
+      <c r="G34" s="12">
+        <v>98418</v>
+      </c>
+      <c r="H34" s="12">
+        <v>109044</v>
+      </c>
+      <c r="I34" s="12">
         <v>49037</v>
       </c>
-      <c r="E34" s="12">
+      <c r="J34" s="12">
         <v>242153</v>
       </c>
-      <c r="F34" s="12">
+      <c r="K34" s="12">
         <v>275951</v>
       </c>
-      <c r="G34" s="12">
+      <c r="L34" s="12">
         <v>689207</v>
       </c>
-      <c r="H34" s="12">
+      <c r="M34" s="12">
         <v>656469</v>
       </c>
     </row>
@@ -1085,19 +1638,40 @@
       <c r="C35" s="16">
         <v/>
       </c>
-      <c r="D35" s="16">
-        <v>0</v>
-      </c>
-      <c r="E35" s="16">
-        <v>0</v>
-      </c>
-      <c r="F35" s="16">
-        <v>0</v>
+      <c r="D35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G35" s="16">
         <v>0</v>
       </c>
       <c r="H35" s="16">
+        <v>0</v>
+      </c>
+      <c r="I35" s="16">
+        <v>0</v>
+      </c>
+      <c r="J35" s="16">
+        <v>0</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0</v>
+      </c>
+      <c r="L35" s="16">
+        <v>0</v>
+      </c>
+      <c r="M35" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1125,6 +1699,21 @@
       <c r="H36" s="12">
         <v>0</v>
       </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>0</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="17" t="inlineStr">
@@ -1136,18 +1725,33 @@
         <v/>
       </c>
       <c r="D37" s="18">
+        <v>344067</v>
+      </c>
+      <c r="E37" s="18">
+        <v>462514</v>
+      </c>
+      <c r="F37" s="18">
+        <v>423191</v>
+      </c>
+      <c r="G37" s="18">
+        <v>592739</v>
+      </c>
+      <c r="H37" s="18">
+        <v>691079</v>
+      </c>
+      <c r="I37" s="18">
         <v>724647</v>
       </c>
-      <c r="E37" s="18">
+      <c r="J37" s="18">
         <v>1235236</v>
       </c>
-      <c r="F37" s="18">
+      <c r="K37" s="18">
         <v>2070164</v>
       </c>
-      <c r="G37" s="18">
+      <c r="L37" s="18">
         <v>3148216</v>
       </c>
-      <c r="H37" s="18">
+      <c r="M37" s="18">
         <v>4681017</v>
       </c>
     </row>
@@ -1175,6 +1779,21 @@
       <c r="H38" s="12">
         <v>0</v>
       </c>
+      <c r="I38" s="12">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12">
+        <v>0</v>
+      </c>
+      <c r="K38" s="12">
+        <v>0</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0</v>
+      </c>
+      <c r="M38" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" s="15" t="inlineStr">
@@ -1185,8 +1804,10 @@
       <c r="C39" s="16">
         <v/>
       </c>
-      <c r="D39" s="16">
-        <v>0</v>
+      <c r="D39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E39" s="16" t="inlineStr">
         <is>
@@ -1198,12 +1819,31 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G39" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H39" s="16" t="inlineStr">
+      <c r="G39" s="16">
+        <v>0</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="16">
+        <v>0</v>
+      </c>
+      <c r="J39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M39" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1219,18 +1859,33 @@
         <v/>
       </c>
       <c r="D40" s="12">
+        <v>0</v>
+      </c>
+      <c r="E40" s="12">
+        <v>0</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0</v>
+      </c>
+      <c r="G40" s="12">
+        <v>0</v>
+      </c>
+      <c r="H40" s="12">
+        <v>20171</v>
+      </c>
+      <c r="I40" s="12">
         <v>19837</v>
       </c>
-      <c r="E40" s="12">
+      <c r="J40" s="12">
         <v>10511</v>
       </c>
-      <c r="F40" s="12">
+      <c r="K40" s="12">
         <v>4222</v>
       </c>
-      <c r="G40" s="12">
+      <c r="L40" s="12">
         <v>19226</v>
       </c>
-      <c r="H40" s="12">
+      <c r="M40" s="12">
         <v>392660</v>
       </c>
     </row>
@@ -1244,18 +1899,33 @@
         <v/>
       </c>
       <c r="D41" s="16">
+        <v>17994</v>
+      </c>
+      <c r="E41" s="16">
+        <v>14826</v>
+      </c>
+      <c r="F41" s="16">
+        <v>22221</v>
+      </c>
+      <c r="G41" s="16">
+        <v>30391</v>
+      </c>
+      <c r="H41" s="16">
+        <v>38044</v>
+      </c>
+      <c r="I41" s="16">
         <v>47884</v>
       </c>
-      <c r="E41" s="16">
+      <c r="J41" s="16">
         <v>63713</v>
       </c>
-      <c r="F41" s="16">
+      <c r="K41" s="16">
         <v>100031</v>
       </c>
-      <c r="G41" s="16">
+      <c r="L41" s="16">
         <v>143955</v>
       </c>
-      <c r="H41" s="16">
+      <c r="M41" s="16">
         <v>214840</v>
       </c>
     </row>
@@ -1269,18 +1939,33 @@
         <v/>
       </c>
       <c r="D42" s="20">
+        <v>17994</v>
+      </c>
+      <c r="E42" s="20">
+        <v>14826</v>
+      </c>
+      <c r="F42" s="20">
+        <v>22221</v>
+      </c>
+      <c r="G42" s="20">
+        <v>30391</v>
+      </c>
+      <c r="H42" s="20">
+        <v>58215</v>
+      </c>
+      <c r="I42" s="20">
         <v>67721</v>
       </c>
-      <c r="E42" s="20">
+      <c r="J42" s="20">
         <v>74224</v>
       </c>
-      <c r="F42" s="20">
+      <c r="K42" s="20">
         <v>104253</v>
       </c>
-      <c r="G42" s="20">
+      <c r="L42" s="20">
         <v>163181</v>
       </c>
-      <c r="H42" s="20">
+      <c r="M42" s="20">
         <v>607500</v>
       </c>
     </row>
@@ -1294,18 +1979,33 @@
         <v/>
       </c>
       <c r="D43" s="18">
+        <v>362061</v>
+      </c>
+      <c r="E43" s="18">
+        <v>477340</v>
+      </c>
+      <c r="F43" s="18">
+        <v>445412</v>
+      </c>
+      <c r="G43" s="18">
+        <v>623130</v>
+      </c>
+      <c r="H43" s="18">
+        <v>749294</v>
+      </c>
+      <c r="I43" s="18">
         <v>792368</v>
       </c>
-      <c r="E43" s="18">
+      <c r="J43" s="18">
         <v>1309460</v>
       </c>
-      <c r="F43" s="18">
+      <c r="K43" s="18">
         <v>2174417</v>
       </c>
-      <c r="G43" s="18">
+      <c r="L43" s="18">
         <v>3311397</v>
       </c>
-      <c r="H43" s="18">
+      <c r="M43" s="18">
         <v>5288517</v>
       </c>
     </row>
@@ -1333,6 +2033,21 @@
       <c r="H44" s="14">
         <v/>
       </c>
+      <c r="I44" s="14">
+        <v/>
+      </c>
+      <c r="J44" s="14">
+        <v/>
+      </c>
+      <c r="K44" s="14">
+        <v/>
+      </c>
+      <c r="L44" s="14">
+        <v/>
+      </c>
+      <c r="M44" s="14">
+        <v/>
+      </c>
     </row>
     <row r="45">
       <c r="B45" s="15" t="inlineStr">
@@ -1344,18 +2059,33 @@
         <v/>
       </c>
       <c r="D45" s="16">
+        <v>84000</v>
+      </c>
+      <c r="E45" s="16">
+        <v>84000</v>
+      </c>
+      <c r="F45" s="16">
+        <v>84000</v>
+      </c>
+      <c r="G45" s="16">
+        <v>84000</v>
+      </c>
+      <c r="H45" s="16">
+        <v>84000</v>
+      </c>
+      <c r="I45" s="16">
         <v>200000</v>
       </c>
-      <c r="E45" s="16">
+      <c r="J45" s="16">
         <v>200000</v>
       </c>
-      <c r="F45" s="16">
+      <c r="K45" s="16">
         <v>226509</v>
       </c>
-      <c r="G45" s="16">
+      <c r="L45" s="16">
         <v>835821</v>
       </c>
-      <c r="H45" s="16">
+      <c r="M45" s="16">
         <v>835821</v>
       </c>
     </row>
@@ -1383,6 +2113,21 @@
       <c r="H46" s="12">
         <v>0</v>
       </c>
+      <c r="I46" s="12">
+        <v>0</v>
+      </c>
+      <c r="J46" s="12">
+        <v>0</v>
+      </c>
+      <c r="K46" s="12">
+        <v>0</v>
+      </c>
+      <c r="L46" s="12">
+        <v>0</v>
+      </c>
+      <c r="M46" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="15" t="inlineStr">
@@ -1397,15 +2142,32 @@
         <v>0</v>
       </c>
       <c r="E47" s="16">
+        <v>0</v>
+      </c>
+      <c r="F47" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" s="16">
+        <v>0</v>
+      </c>
+      <c r="H47" s="16">
+        <v>114441</v>
+      </c>
+      <c r="I47" s="16">
+        <v>0</v>
+      </c>
+      <c r="J47" s="16">
         <v>26509</v>
       </c>
-      <c r="F47" s="16">
-        <v>0</v>
-      </c>
-      <c r="G47" s="16">
-        <v>0</v>
-      </c>
-      <c r="H47" s="16">
+      <c r="K47" s="16">
+        <v>0</v>
+      </c>
+      <c r="L47" s="16">
+        <v>0</v>
+      </c>
+      <c r="M47" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1418,11 +2180,15 @@
       <c r="C48" s="12">
         <v/>
       </c>
-      <c r="D48" s="12">
-        <v>0</v>
-      </c>
-      <c r="E48" s="12">
-        <v>0</v>
+      <c r="D48" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F48" s="12">
         <v>0</v>
@@ -1431,6 +2197,21 @@
         <v>0</v>
       </c>
       <c r="H48" s="12">
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <v>0</v>
+      </c>
+      <c r="J48" s="12">
+        <v>0</v>
+      </c>
+      <c r="K48" s="12">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
+        <v>0</v>
+      </c>
+      <c r="M48" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1448,16 +2229,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E49" s="16">
-        <v>0</v>
-      </c>
-      <c r="F49" s="16">
-        <v>0</v>
-      </c>
-      <c r="G49" s="16">
-        <v>0</v>
-      </c>
-      <c r="H49" s="16">
+      <c r="E49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J49" s="16">
+        <v>0</v>
+      </c>
+      <c r="K49" s="16">
+        <v>0</v>
+      </c>
+      <c r="L49" s="16">
+        <v>0</v>
+      </c>
+      <c r="M49" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1471,18 +2277,33 @@
         <v/>
       </c>
       <c r="D50" s="12">
+        <v>8400</v>
+      </c>
+      <c r="E50" s="12">
+        <v>8400</v>
+      </c>
+      <c r="F50" s="12">
+        <v>8400</v>
+      </c>
+      <c r="G50" s="12">
+        <v>8400</v>
+      </c>
+      <c r="H50" s="12">
+        <v>13800</v>
+      </c>
+      <c r="I50" s="12">
         <v>20000</v>
       </c>
-      <c r="E50" s="12">
+      <c r="J50" s="12">
         <v>20000</v>
       </c>
-      <c r="F50" s="12">
+      <c r="K50" s="12">
         <v>22651</v>
       </c>
-      <c r="G50" s="12">
+      <c r="L50" s="12">
         <v>50693</v>
       </c>
-      <c r="H50" s="12">
+      <c r="M50" s="12">
         <v>83582</v>
       </c>
     </row>
@@ -1510,6 +2331,21 @@
       <c r="H51" s="16">
         <v>0</v>
       </c>
+      <c r="I51" s="16">
+        <v>0</v>
+      </c>
+      <c r="J51" s="16">
+        <v>0</v>
+      </c>
+      <c r="K51" s="16">
+        <v>0</v>
+      </c>
+      <c r="L51" s="16">
+        <v>0</v>
+      </c>
+      <c r="M51" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="11" t="inlineStr">
@@ -1523,22 +2359,37 @@
       <c r="D52" s="12">
         <v>0</v>
       </c>
-      <c r="E52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H52" s="12" t="inlineStr">
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <v>0</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0</v>
+      </c>
+      <c r="H52" s="12">
+        <v>0</v>
+      </c>
+      <c r="I52" s="12">
+        <v>0</v>
+      </c>
+      <c r="J52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M52" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1560,12 +2411,27 @@
         <v>0</v>
       </c>
       <c r="F53" s="16">
+        <v>0</v>
+      </c>
+      <c r="G53" s="16">
+        <v>0</v>
+      </c>
+      <c r="H53" s="16">
+        <v>0</v>
+      </c>
+      <c r="I53" s="16">
+        <v>0</v>
+      </c>
+      <c r="J53" s="16">
+        <v>0</v>
+      </c>
+      <c r="K53" s="16">
         <v>609312</v>
       </c>
-      <c r="G53" s="16">
-        <v>0</v>
-      </c>
-      <c r="H53" s="16">
+      <c r="L53" s="16">
+        <v>0</v>
+      </c>
+      <c r="M53" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1581,22 +2447,37 @@
       <c r="D54" s="12">
         <v>0</v>
       </c>
-      <c r="E54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H54" s="12" t="inlineStr">
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0</v>
+      </c>
+      <c r="H54" s="12">
+        <v>0</v>
+      </c>
+      <c r="I54" s="12">
+        <v>0</v>
+      </c>
+      <c r="J54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M54" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1611,19 +2492,40 @@
       <c r="C55" s="16">
         <v/>
       </c>
-      <c r="D55" s="16">
-        <v>0</v>
-      </c>
-      <c r="E55" s="16">
-        <v>0</v>
-      </c>
-      <c r="F55" s="16">
-        <v>0</v>
+      <c r="D55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G55" s="16">
         <v>0</v>
       </c>
       <c r="H55" s="16">
+        <v>0</v>
+      </c>
+      <c r="I55" s="16">
+        <v>0</v>
+      </c>
+      <c r="J55" s="16">
+        <v>0</v>
+      </c>
+      <c r="K55" s="16">
+        <v>0</v>
+      </c>
+      <c r="L55" s="16">
+        <v>0</v>
+      </c>
+      <c r="M55" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1637,18 +2539,33 @@
         <v/>
       </c>
       <c r="D56" s="12">
+        <v>81838</v>
+      </c>
+      <c r="E56" s="12">
+        <v>69739</v>
+      </c>
+      <c r="F56" s="12">
+        <v>106518</v>
+      </c>
+      <c r="G56" s="12">
+        <v>124962</v>
+      </c>
+      <c r="H56" s="12">
+        <v>169698</v>
+      </c>
+      <c r="I56" s="12">
         <v>212660</v>
       </c>
-      <c r="E56" s="12">
+      <c r="J56" s="12">
         <v>277230</v>
       </c>
-      <c r="F56" s="12">
+      <c r="K56" s="12">
         <v>465507</v>
       </c>
-      <c r="G56" s="12">
+      <c r="L56" s="12">
         <v>689056</v>
       </c>
-      <c r="H56" s="12">
+      <c r="M56" s="12">
         <v>1099327</v>
       </c>
     </row>
@@ -1662,18 +2579,33 @@
         <v/>
       </c>
       <c r="D57" s="18">
+        <v>174238</v>
+      </c>
+      <c r="E57" s="18">
+        <v>162139</v>
+      </c>
+      <c r="F57" s="18">
+        <v>198918</v>
+      </c>
+      <c r="G57" s="18">
+        <v>217362</v>
+      </c>
+      <c r="H57" s="18">
+        <v>381939</v>
+      </c>
+      <c r="I57" s="18">
         <v>432660</v>
       </c>
-      <c r="E57" s="18">
+      <c r="J57" s="18">
         <v>523739</v>
       </c>
-      <c r="F57" s="18">
+      <c r="K57" s="18">
         <v>1323979</v>
       </c>
-      <c r="G57" s="18">
+      <c r="L57" s="18">
         <v>1575570</v>
       </c>
-      <c r="H57" s="18">
+      <c r="M57" s="18">
         <v>2018730</v>
       </c>
     </row>
@@ -1687,18 +2619,33 @@
         <v/>
       </c>
       <c r="D58" s="20">
+        <v>536299</v>
+      </c>
+      <c r="E58" s="20">
+        <v>639479</v>
+      </c>
+      <c r="F58" s="20">
+        <v>644330</v>
+      </c>
+      <c r="G58" s="20">
+        <v>840492</v>
+      </c>
+      <c r="H58" s="20">
+        <v>1131233</v>
+      </c>
+      <c r="I58" s="20">
         <v>1225028</v>
       </c>
-      <c r="E58" s="20">
+      <c r="J58" s="20">
         <v>1833199</v>
       </c>
-      <c r="F58" s="20">
+      <c r="K58" s="20">
         <v>3498396</v>
       </c>
-      <c r="G58" s="20">
+      <c r="L58" s="20">
         <v>4886967</v>
       </c>
-      <c r="H58" s="20">
+      <c r="M58" s="20">
         <v>7307247</v>
       </c>
     </row>
@@ -1722,6 +2669,21 @@
         <v/>
       </c>
       <c r="H59" s="2">
+        <v/>
+      </c>
+      <c r="I59" s="2">
+        <v/>
+      </c>
+      <c r="J59" s="2">
+        <v/>
+      </c>
+      <c r="K59" s="2">
+        <v/>
+      </c>
+      <c r="L59" s="2">
+        <v/>
+      </c>
+      <c r="M59" s="2">
         <v/>
       </c>
     </row>

</xml_diff>